<commit_message>
Update IP - EX 49 - Super exercicio III (Anexo).xlsx
Primeira parte da lógica montada.
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 49 - Super exercicio III (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 49 - Super exercicio III (Anexo).xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E62456F3-79CE-46CC-8095-317FCF049755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876EE434-FE84-4F69-B2A4-AB3035705526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
     <sheet name="EXERCÍCIO" sheetId="4" r:id="rId2"/>
-    <sheet name="EXERCÍCIO-RESOLVIDO" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="Planilha1" sheetId="6" state="hidden" r:id="rId3"/>
+    <sheet name="EXERCÍCIO-RESOLVIDO" sheetId="5" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,8 +32,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
   <si>
     <t>Manufatura</t>
   </si>
@@ -113,12 +136,6 @@
   </si>
   <si>
     <t>TOTAL (SEM DESCONTO)</t>
-  </si>
-  <si>
-    <t>MANUFATURA</t>
-  </si>
-  <si>
-    <t>TORNO</t>
   </si>
   <si>
     <t>EXERCÍCIO</t>
@@ -161,9 +178,6 @@
 Automaticamente deverá sair o valor total (valor unitário*quantidade). No entanto, caso não tenha quantidade desejada em estoque, deve ser alertado através de uma mensagem (ALERTA DE ESTOQUE!). Qualquer erro deve ser avisado para usuário verificar o preenchimento. 
 Utilize a tabela de descontos abaixo como base de cálculo; e insira uma formatação condicional por tipo, conforme tabela abaixo, para deixar visualmente fácil a interepretação do pedido. 
 Faça o exercício na aba Exercício.</t>
-  </si>
-  <si>
-    <t>ALERTA DE ERRO!</t>
   </si>
   <si>
     <t>*resolução = aba oculta</t>
@@ -705,7 +719,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -978,6 +992,13 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1579,7 +1600,7 @@
   <dimension ref="B1:Q26"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:Q15"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,7 +1608,7 @@
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -1679,7 +1700,7 @@
     </row>
     <row r="8" spans="2:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
@@ -1703,7 +1724,7 @@
     </row>
     <row r="10" spans="2:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
@@ -1813,20 +1834,20 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="16"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C19" s="18"/>
       <c r="D19" s="19">
@@ -1835,7 +1856,7 @@
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="19">
@@ -1844,7 +1865,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C21" s="21"/>
       <c r="D21" s="22">
@@ -1854,7 +1875,7 @@
     <row r="22" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1862,7 +1883,7 @@
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -1870,7 +1891,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -1878,7 +1899,7 @@
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
@@ -1896,10 +1917,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B1:Q31"/>
+  <dimension ref="B1:Q45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,13 +1928,15 @@
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
@@ -2005,7 +2028,7 @@
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="P7" s="29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -2177,7 +2200,7 @@
     <row r="16" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C17" s="68"/>
       <c r="D17" s="68"/>
@@ -2226,14 +2249,15 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="27">
+        <f>IF(C21&lt;&gt;"",1,"")</f>
         <v>1</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D21" s="58"/>
       <c r="E21" s="59" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="F21" s="60"/>
       <c r="G21" s="61"/>
@@ -2241,21 +2265,23 @@
         <v>1</v>
       </c>
       <c r="I21" s="58"/>
-      <c r="J21" s="62">
-        <v>9000</v>
-      </c>
-      <c r="K21" s="62"/>
+      <c r="J21" s="109" cm="1">
+        <f t="array" ref="J21">_xlfn.IFS($C21=$B$8,IF(VLOOKUP($E21,$B$9:$D$15,2,FALSE)&gt;=$H21,VLOOKUP($E21,$B$9:$D$15,3,FALSE)*$H21,"Qtd fora de estoque!"))</f>
+        <v>50000</v>
+      </c>
+      <c r="K21" s="109"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="28">
+        <f>IF(C22&lt;&gt;"",B21+1,"")</f>
         <v>2</v>
       </c>
       <c r="C22" s="53" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D22" s="53"/>
       <c r="E22" s="54" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="F22" s="55"/>
       <c r="G22" s="56"/>
@@ -2263,46 +2289,59 @@
         <v>2</v>
       </c>
       <c r="I22" s="53"/>
-      <c r="J22" s="53" t="s">
-        <v>42</v>
-      </c>
+      <c r="J22" s="53"/>
       <c r="K22" s="53"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="27"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="58"/>
+      <c r="B23" s="27">
+        <f t="shared" ref="B23:B28" si="0">IF(C23&lt;&gt;"",B22+1,"")</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="61"/>
       <c r="E23" s="59" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F23" s="60"/>
       <c r="G23" s="61"/>
-      <c r="H23" s="58"/>
+      <c r="H23" s="58">
+        <v>1</v>
+      </c>
       <c r="I23" s="58"/>
       <c r="J23" s="63"/>
       <c r="K23" s="64"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53"/>
+      <c r="B24" s="28">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="56"/>
       <c r="E24" s="54" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="F24" s="55"/>
       <c r="G24" s="56"/>
-      <c r="H24" s="53"/>
+      <c r="H24" s="53">
+        <v>2</v>
+      </c>
       <c r="I24" s="53"/>
       <c r="J24" s="53"/>
       <c r="K24" s="53"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="27"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="59" t="s">
-        <v>28</v>
-      </c>
+      <c r="B25" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="60"/>
       <c r="G25" s="61"/>
       <c r="H25" s="58"/>
@@ -2311,12 +2350,13 @@
       <c r="K25" s="64"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="54" t="s">
-        <v>28</v>
-      </c>
+      <c r="B26" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C26" s="54"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="55"/>
       <c r="G26" s="56"/>
       <c r="H26" s="53"/>
@@ -2325,12 +2365,13 @@
       <c r="K26" s="53"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="27"/>
-      <c r="C27" s="58"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59" t="s">
-        <v>28</v>
-      </c>
+      <c r="B27" s="27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C27" s="59"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="59"/>
       <c r="F27" s="60"/>
       <c r="G27" s="61"/>
       <c r="H27" s="58"/>
@@ -2339,12 +2380,13 @@
       <c r="K27" s="62"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="54" t="s">
-        <v>28</v>
-      </c>
+      <c r="B28" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C28" s="54"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="55"/>
       <c r="G28" s="56"/>
       <c r="H28" s="53"/>
@@ -2375,6 +2417,98 @@
       <c r="I31" s="51"/>
       <c r="J31" s="52"/>
       <c r="K31" s="52"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="str" cm="1">
+        <f t="array" ref="F34:F39">_xlfn.IFS($C21=$B$8,$B$10:$B$15,$C21=$F$8,$F$10:$F$13,$C21=$J$8,$J$10:$J$11)</f>
+        <v>Husky</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F35" t="str">
+        <v>Torno</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F36" t="str">
+        <v>CNC</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16"/>
+      <c r="F37" t="str">
+        <v>Fresadora</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="19">
+        <v>0.04</v>
+      </c>
+      <c r="F38" t="str">
+        <v>Forno 1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F39" t="str">
+        <v>Roletes</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="21"/>
+      <c r="D40" s="22">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="23"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="23"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="47">
@@ -2426,17 +2560,72 @@
     <mergeCell ref="H29:I29"/>
     <mergeCell ref="J29:K29"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E21:G28" xr:uid="{84D5CEAF-9DEF-4602-B57D-7BA1C93CCCCD}">
+      <formula1>_xlfn.IFS($C21=$B$8,$B$10:$B$15,$C21=$F$8,$F$10:$F$13,$C21=$J$8,$J$10:$J$11)</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE99BD4A-825F-469F-8A41-380EE66608CB}">
+          <x14:formula1>
+            <xm:f>Planilha1!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C21:D28</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445A2AE9-907C-4CA4-B079-9F735774085D}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" style="107" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="108" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="108" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="108" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:Q31"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>